<commit_message>
Added MAP to the whole system without 1 query
</commit_message>
<xml_diff>
--- a/solr/EvaluationM3.xlsx
+++ b/solr/EvaluationM3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Documents\GitHub\PRI\solr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\PRI\solr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C09115-FA96-4B8A-83FF-B86122CD623A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EE1B50-A87F-438F-848D-9BFB68828424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1F5A3B19-910C-4A1F-9359-A2D6231D0330}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="21">
   <si>
     <t>Rank</t>
   </si>
@@ -106,10 +106,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,7 +206,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -224,6 +225,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2842,7 +2844,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$4:$V$14</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2950,7 +2952,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$4:$V$14</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -3206,7 +3208,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3428,7 +3430,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$20:$V$30</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -3536,7 +3538,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$20:$V$30</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -3806,7 +3808,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4096,7 +4098,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$4:$V$14</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -4204,7 +4206,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$4:$V$14</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -4460,7 +4462,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4660,7 +4662,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$4:$V$14</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -4768,7 +4770,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$4:$V$14</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -5024,7 +5026,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5224,7 +5226,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$4:$V$14</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -5332,7 +5334,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$4:$V$14</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -5588,7 +5590,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5810,7 +5812,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$20:$V$30</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -5918,7 +5920,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$20:$V$30</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -6188,7 +6190,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7463,7 +7465,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$4:$V$14</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -7571,7 +7573,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$4:$V$14</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -7827,7 +7829,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -8049,7 +8051,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$20:$V$30</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -8157,7 +8159,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$20:$V$30</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -8427,7 +8429,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -10620,7 +10622,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$4:$V$14</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -10728,7 +10730,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$4:$V$14</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -10984,7 +10986,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -11206,7 +11208,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$20:$V$30</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -11314,7 +11316,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$V$20:$V$30</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -11584,7 +11586,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -12285,9 +12287,6 @@
           <cell r="W3" t="str">
             <v>V1</v>
           </cell>
-          <cell r="X3" t="str">
-            <v>V2</v>
-          </cell>
         </row>
         <row r="4">
           <cell r="A4">
@@ -12503,378 +12502,6 @@
         <row r="33">
           <cell r="A33">
             <v>30</v>
-          </cell>
-        </row>
-        <row r="139">
-          <cell r="J139">
-            <v>1</v>
-          </cell>
-          <cell r="K139">
-            <v>1</v>
-          </cell>
-          <cell r="W139">
-            <v>1</v>
-          </cell>
-          <cell r="X139">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="140">
-          <cell r="J140">
-            <v>1</v>
-          </cell>
-          <cell r="K140">
-            <v>1</v>
-          </cell>
-          <cell r="W140">
-            <v>1</v>
-          </cell>
-          <cell r="X140">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="141">
-          <cell r="J141">
-            <v>0.66666666666666663</v>
-          </cell>
-          <cell r="K141">
-            <v>1</v>
-          </cell>
-          <cell r="W141">
-            <v>1</v>
-          </cell>
-          <cell r="X141">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="142">
-          <cell r="J142">
-            <v>0.5</v>
-          </cell>
-          <cell r="K142">
-            <v>1</v>
-          </cell>
-          <cell r="W142">
-            <v>1</v>
-          </cell>
-          <cell r="X142">
-            <v>0.83333333333333337</v>
-          </cell>
-        </row>
-        <row r="143">
-          <cell r="J143">
-            <v>0.6</v>
-          </cell>
-          <cell r="K143">
-            <v>0.8</v>
-          </cell>
-          <cell r="W143">
-            <v>1</v>
-          </cell>
-          <cell r="X143">
-            <v>0.7</v>
-          </cell>
-        </row>
-        <row r="144">
-          <cell r="J144">
-            <v>0.5</v>
-          </cell>
-          <cell r="K144">
-            <v>0.83333333333333337</v>
-          </cell>
-          <cell r="W144">
-            <v>0.6</v>
-          </cell>
-          <cell r="X144">
-            <v>0.61904761904761907</v>
-          </cell>
-        </row>
-        <row r="145">
-          <cell r="J145">
-            <v>0.42857142857142855</v>
-          </cell>
-          <cell r="K145">
-            <v>0.7142857142857143</v>
-          </cell>
-          <cell r="W145">
-            <v>0.6</v>
-          </cell>
-          <cell r="X145">
-            <v>0.61904761904761907</v>
-          </cell>
-        </row>
-        <row r="146">
-          <cell r="J146">
-            <v>0.375</v>
-          </cell>
-          <cell r="K146">
-            <v>0.625</v>
-          </cell>
-          <cell r="W146">
-            <v>0.4</v>
-          </cell>
-          <cell r="X146">
-            <v>0.61904761904761907</v>
-          </cell>
-        </row>
-        <row r="147">
-          <cell r="J147">
-            <v>0.33333333333333331</v>
-          </cell>
-          <cell r="K147">
-            <v>0.66666666666666663</v>
-          </cell>
-          <cell r="W147">
-            <v>0.4</v>
-          </cell>
-          <cell r="X147">
-            <v>0.61904761904761907</v>
-          </cell>
-        </row>
-        <row r="148">
-          <cell r="J148">
-            <v>0.4</v>
-          </cell>
-          <cell r="K148">
-            <v>0.7</v>
-          </cell>
-          <cell r="W148">
-            <v>0.33333333333333331</v>
-          </cell>
-          <cell r="X148">
-            <v>0.60869565217391308</v>
-          </cell>
-        </row>
-        <row r="149">
-          <cell r="J149">
-            <v>0.36363636363636365</v>
-          </cell>
-          <cell r="K149">
-            <v>0.63636363636363635</v>
-          </cell>
-          <cell r="W149">
-            <v>0.33333333333333331</v>
-          </cell>
-          <cell r="X149">
-            <v>0.57692307692307687</v>
-          </cell>
-        </row>
-        <row r="150">
-          <cell r="J150">
-            <v>0.33333333333333331</v>
-          </cell>
-          <cell r="K150">
-            <v>0.58333333333333337</v>
-          </cell>
-        </row>
-        <row r="151">
-          <cell r="J151">
-            <v>0.30769230769230771</v>
-          </cell>
-          <cell r="K151">
-            <v>0.53846153846153844</v>
-          </cell>
-        </row>
-        <row r="152">
-          <cell r="J152">
-            <v>0.2857142857142857</v>
-          </cell>
-          <cell r="K152">
-            <v>0.5</v>
-          </cell>
-        </row>
-        <row r="153">
-          <cell r="J153">
-            <v>0.33333333333333331</v>
-          </cell>
-          <cell r="K153">
-            <v>0.53333333333333333</v>
-          </cell>
-        </row>
-        <row r="154">
-          <cell r="J154">
-            <v>0.3125</v>
-          </cell>
-          <cell r="K154">
-            <v>0.5625</v>
-          </cell>
-        </row>
-        <row r="155">
-          <cell r="J155">
-            <v>0.29411764705882354</v>
-          </cell>
-          <cell r="K155">
-            <v>0.52941176470588236</v>
-          </cell>
-          <cell r="W155">
-            <v>0</v>
-          </cell>
-          <cell r="X155">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="156">
-          <cell r="J156">
-            <v>0.27777777777777779</v>
-          </cell>
-          <cell r="K156">
-            <v>0.55555555555555558</v>
-          </cell>
-          <cell r="W156">
-            <v>0.18181818181818182</v>
-          </cell>
-          <cell r="X156">
-            <v>0.18181818181818182</v>
-          </cell>
-        </row>
-        <row r="157">
-          <cell r="J157">
-            <v>0.26315789473684209</v>
-          </cell>
-          <cell r="K157">
-            <v>0.57894736842105265</v>
-          </cell>
-          <cell r="W157">
-            <v>0.33333333333333337</v>
-          </cell>
-          <cell r="X157">
-            <v>0.33333333333333337</v>
-          </cell>
-        </row>
-        <row r="158">
-          <cell r="J158">
-            <v>0.25</v>
-          </cell>
-          <cell r="K158">
-            <v>0.6</v>
-          </cell>
-          <cell r="W158">
-            <v>0.46153846153846151</v>
-          </cell>
-          <cell r="X158">
-            <v>0.44117647058823528</v>
-          </cell>
-        </row>
-        <row r="159">
-          <cell r="J159">
-            <v>0.23809523809523808</v>
-          </cell>
-          <cell r="K159">
-            <v>0.61904761904761907</v>
-          </cell>
-          <cell r="W159">
-            <v>0.57142857142857151</v>
-          </cell>
-          <cell r="X159">
-            <v>0.50909090909090904</v>
-          </cell>
-        </row>
-        <row r="160">
-          <cell r="J160">
-            <v>0.22727272727272727</v>
-          </cell>
-          <cell r="K160">
-            <v>0.59090909090909094</v>
-          </cell>
-          <cell r="W160">
-            <v>0.54545454545454541</v>
-          </cell>
-          <cell r="X160">
-            <v>0.55319148936170215</v>
-          </cell>
-        </row>
-        <row r="161">
-          <cell r="J161">
-            <v>0.21739130434782608</v>
-          </cell>
-          <cell r="K161">
-            <v>0.60869565217391308</v>
-          </cell>
-          <cell r="W161">
-            <v>0.6</v>
-          </cell>
-          <cell r="X161">
-            <v>0.609375</v>
-          </cell>
-        </row>
-        <row r="162">
-          <cell r="J162">
-            <v>0.20833333333333334</v>
-          </cell>
-          <cell r="K162">
-            <v>0.58333333333333337</v>
-          </cell>
-          <cell r="W162">
-            <v>0.50909090909090904</v>
-          </cell>
-          <cell r="X162">
-            <v>0.65703971119133575</v>
-          </cell>
-        </row>
-        <row r="163">
-          <cell r="J163">
-            <v>0.2</v>
-          </cell>
-          <cell r="K163">
-            <v>0.56000000000000005</v>
-          </cell>
-          <cell r="W163">
-            <v>0.53333333333333333</v>
-          </cell>
-          <cell r="X163">
-            <v>0.69798657718120805</v>
-          </cell>
-        </row>
-        <row r="164">
-          <cell r="J164">
-            <v>0.19230769230769232</v>
-          </cell>
-          <cell r="K164">
-            <v>0.57692307692307687</v>
-          </cell>
-          <cell r="W164">
-            <v>0.48648648648648646</v>
-          </cell>
-          <cell r="X164">
-            <v>0.72622478386167155</v>
-          </cell>
-        </row>
-        <row r="165">
-          <cell r="J165">
-            <v>0.18518518518518517</v>
-          </cell>
-          <cell r="K165">
-            <v>0.55555555555555558</v>
-          </cell>
-          <cell r="W165">
-            <v>0.5</v>
-          </cell>
-          <cell r="X165">
-            <v>0.73170731707317072</v>
-          </cell>
-        </row>
-        <row r="166">
-          <cell r="J166">
-            <v>0.17857142857142858</v>
-          </cell>
-          <cell r="K166">
-            <v>0.5357142857142857</v>
-          </cell>
-        </row>
-        <row r="167">
-          <cell r="J167">
-            <v>0.17241379310344829</v>
-          </cell>
-          <cell r="K167">
-            <v>0.51724137931034486</v>
-          </cell>
-        </row>
-        <row r="168">
-          <cell r="J168">
-            <v>0.16666666666666666</v>
-          </cell>
-          <cell r="K168">
-            <v>0.5</v>
           </cell>
         </row>
       </sheetData>
@@ -13182,20 +12809,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90E2CE5-2754-4DEC-9740-5E5101C42739}">
   <dimension ref="A1:AC211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X207" sqref="X207"/>
+    <sheetView tabSelected="1" topLeftCell="A176" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H207" sqref="H207"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="25" width="9.140625" style="1"/>
     <col min="26" max="26" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -13203,7 +12830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:29" ht="15">
       <c r="J2" s="9" t="s">
         <v>7</v>
       </c>
@@ -13235,7 +12862,7 @@
       <c r="AB2" s="9"/>
       <c r="AC2" s="9"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:29">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -13303,7 +12930,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:29">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -13387,7 +13014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:29">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -13471,7 +13098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:29">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -13555,7 +13182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:29">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -13639,7 +13266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:29">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -13723,7 +13350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:29">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -13807,7 +13434,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:29">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -13891,7 +13518,7 @@
         <v>0.6470588235294118</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:29">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -13975,7 +13602,7 @@
         <v>0.63157894736842102</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:29">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -14059,7 +13686,7 @@
         <v>0.58620689655172409</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:29">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -14143,7 +13770,7 @@
         <v>0.58620689655172409</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:29">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -14227,7 +13854,7 @@
         <v>0.58620689655172409</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:29">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -14292,7 +13919,7 @@
         <v>0.52941176470588236</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:29">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -14357,7 +13984,7 @@
         <v>0.52941176470588236</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:29">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -14422,7 +14049,7 @@
         <v>0.52941176470588236</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:29">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -14493,7 +14120,7 @@
       <c r="AB18" s="9"/>
       <c r="AC18" s="9"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:29">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -14573,7 +14200,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:29">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -14657,7 +14284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:29">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -14741,7 +14368,7 @@
         <v>0.18181818181818182</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:29">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -14825,7 +14452,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:29">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -14909,7 +14536,7 @@
         <v>0.46153846153846151</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:29">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -14993,7 +14620,7 @@
         <v>0.57142857142857151</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:29">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -15077,7 +14704,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:29">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -15161,7 +14788,7 @@
         <v>0.62264150943396224</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:29">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -15245,7 +14872,7 @@
         <v>0.66403162055335962</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:29">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -15329,7 +14956,7 @@
         <v>0.6766169154228856</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:29">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -15413,7 +15040,7 @@
         <v>0.7099767981438514</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:29">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -15497,7 +15124,7 @@
         <v>0.73913043478260865</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:29">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -15562,7 +15189,7 @@
         <v>0.94117647058823528</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:29">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -15627,7 +15254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:29">
       <c r="A33" s="1">
         <v>30</v>
       </c>
@@ -15692,7 +15319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:29" ht="15">
       <c r="I34" s="5" t="s">
         <v>8</v>
       </c>
@@ -15713,12 +15340,12 @@
         <v>0.72710483381485191</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:29">
       <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:29" ht="15" customHeight="1">
       <c r="J37" s="9" t="s">
         <v>7</v>
       </c>
@@ -15746,7 +15373,7 @@
       <c r="AB37" s="9"/>
       <c r="AC37" s="9"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:29">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
@@ -15814,7 +15441,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:29">
       <c r="A39" s="1">
         <v>1</v>
       </c>
@@ -15898,7 +15525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:29">
       <c r="A40" s="1">
         <v>2</v>
       </c>
@@ -15982,7 +15609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:29">
       <c r="A41" s="1">
         <v>3</v>
       </c>
@@ -16066,7 +15693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:29">
       <c r="A42" s="1">
         <v>4</v>
       </c>
@@ -16150,7 +15777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:29">
       <c r="A43" s="1">
         <v>5</v>
       </c>
@@ -16234,7 +15861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:29">
       <c r="A44" s="1">
         <v>6</v>
       </c>
@@ -16318,7 +15945,7 @@
         <v>0.76923076923076927</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:29">
       <c r="A45" s="1">
         <v>7</v>
       </c>
@@ -16402,7 +16029,7 @@
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:29">
       <c r="A46" s="1">
         <v>8</v>
       </c>
@@ -16486,7 +16113,7 @@
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:29">
       <c r="A47" s="1">
         <v>9</v>
       </c>
@@ -16570,7 +16197,7 @@
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:29">
       <c r="A48" s="1">
         <v>10</v>
       </c>
@@ -16654,7 +16281,7 @@
         <v>0.65384615384615385</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:29">
       <c r="A49" s="1">
         <v>11</v>
       </c>
@@ -16738,7 +16365,7 @@
         <v>0.62068965517241381</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:29">
       <c r="A50" s="1">
         <v>12</v>
       </c>
@@ -16803,7 +16430,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:29">
       <c r="A51" s="1">
         <v>13</v>
       </c>
@@ -16868,7 +16495,7 @@
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:29">
       <c r="A52" s="1">
         <v>14</v>
       </c>
@@ -16933,7 +16560,7 @@
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:29">
       <c r="A53" s="1">
         <v>15</v>
       </c>
@@ -17004,7 +16631,7 @@
       <c r="AB53" s="9"/>
       <c r="AC53" s="9"/>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:29">
       <c r="A54" s="1">
         <v>16</v>
       </c>
@@ -17084,7 +16711,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:29">
       <c r="A55" s="1">
         <v>17</v>
       </c>
@@ -17168,7 +16795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:29">
       <c r="A56" s="1">
         <v>18</v>
       </c>
@@ -17252,7 +16879,7 @@
         <v>0.18181818181818182</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:29">
       <c r="A57" s="1">
         <v>19</v>
       </c>
@@ -17336,7 +16963,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:29">
       <c r="A58" s="1">
         <v>20</v>
       </c>
@@ -17420,7 +17047,7 @@
         <v>0.46153846153846151</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:29">
       <c r="A59" s="1">
         <v>21</v>
       </c>
@@ -17504,7 +17131,7 @@
         <v>0.57142857142857151</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:29">
       <c r="A60" s="1">
         <v>22</v>
       </c>
@@ -17588,7 +17215,7 @@
         <v>0.60606060606060608</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:29">
       <c r="A61" s="1">
         <v>23</v>
       </c>
@@ -17672,7 +17299,7 @@
         <v>0.65217391304347827</v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:29">
       <c r="A62" s="1">
         <v>24</v>
       </c>
@@ -17756,7 +17383,7 @@
         <v>0.70707070707070718</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:29">
       <c r="A63" s="1">
         <v>25</v>
       </c>
@@ -17840,7 +17467,7 @@
         <v>0.75471698113207564</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:29">
       <c r="A64" s="1">
         <v>26</v>
       </c>
@@ -17924,7 +17551,7 @@
         <v>0.75742574257425743</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:29">
       <c r="A65" s="1">
         <v>27</v>
       </c>
@@ -18008,7 +17635,7 @@
         <v>0.76595744680851074</v>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:29">
       <c r="A66" s="1">
         <v>28</v>
       </c>
@@ -18073,7 +17700,7 @@
         <v>0.94444444444444442</v>
       </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:29">
       <c r="A67" s="1">
         <v>29</v>
       </c>
@@ -18138,7 +17765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:29">
       <c r="A68" s="1">
         <v>30</v>
       </c>
@@ -18203,7 +17830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:29" ht="15">
       <c r="I69" s="5" t="s">
         <v>8</v>
       </c>
@@ -18224,12 +17851,12 @@
         <v>0.77018445181539108</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:29">
       <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:29" ht="15" customHeight="1">
       <c r="J72" s="9" t="s">
         <v>7</v>
       </c>
@@ -18257,7 +17884,7 @@
       <c r="AB72" s="9"/>
       <c r="AC72" s="9"/>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:29">
       <c r="A73" s="2" t="s">
         <v>0</v>
       </c>
@@ -18325,7 +17952,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:29">
       <c r="A74" s="1">
         <v>1</v>
       </c>
@@ -18409,7 +18036,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:29">
       <c r="A75" s="1">
         <v>2</v>
       </c>
@@ -18493,7 +18120,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:29">
       <c r="A76" s="1">
         <v>3</v>
       </c>
@@ -18577,7 +18204,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:29">
       <c r="A77" s="1">
         <v>4</v>
       </c>
@@ -18661,7 +18288,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:29">
       <c r="A78" s="1">
         <v>5</v>
       </c>
@@ -18745,7 +18372,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:29">
       <c r="A79" s="1">
         <v>6</v>
       </c>
@@ -18829,7 +18456,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:29">
       <c r="A80" s="1">
         <v>7</v>
       </c>
@@ -18913,7 +18540,7 @@
         <v>0.25925925925925924</v>
       </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:29">
       <c r="A81" s="1">
         <v>8</v>
       </c>
@@ -18997,7 +18624,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:29">
       <c r="A82" s="1">
         <v>9</v>
       </c>
@@ -19081,7 +18708,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:29">
       <c r="A83" s="1">
         <v>10</v>
       </c>
@@ -19165,7 +18792,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:29">
       <c r="A84" s="1">
         <v>11</v>
       </c>
@@ -19249,7 +18876,7 @@
         <v>0.18333333333333332</v>
       </c>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:29">
       <c r="A85" s="1">
         <v>12</v>
       </c>
@@ -19314,7 +18941,7 @@
         <v>0.18181818181818182</v>
       </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:29">
       <c r="A86" s="1">
         <v>13</v>
       </c>
@@ -19379,7 +19006,7 @@
         <v>0.18181818181818182</v>
       </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:29">
       <c r="A87" s="1">
         <v>14</v>
       </c>
@@ -19444,7 +19071,7 @@
         <v>0.18181818181818182</v>
       </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:29">
       <c r="A88" s="1">
         <v>15</v>
       </c>
@@ -19515,7 +19142,7 @@
       <c r="AB88" s="9"/>
       <c r="AC88" s="9"/>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:29">
       <c r="A89" s="1">
         <v>16</v>
       </c>
@@ -19595,7 +19222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:29">
       <c r="A90" s="1">
         <v>17</v>
       </c>
@@ -19679,7 +19306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:29">
       <c r="A91" s="1">
         <v>18</v>
       </c>
@@ -19763,7 +19390,7 @@
         <v>0.14814814814814817</v>
       </c>
     </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:29">
       <c r="A92" s="1">
         <v>19</v>
       </c>
@@ -19847,7 +19474,7 @@
         <v>0.23529411764705882</v>
       </c>
     </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:29">
       <c r="A93" s="1">
         <v>20</v>
       </c>
@@ -19931,7 +19558,7 @@
         <v>0.29268292682926828</v>
       </c>
     </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:29">
       <c r="A94" s="1">
         <v>21</v>
       </c>
@@ -20015,7 +19642,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:29">
       <c r="A95" s="1">
         <v>22</v>
       </c>
@@ -20099,7 +19726,7 @@
         <v>0.36363636363636365</v>
       </c>
     </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:29">
       <c r="A96" s="1">
         <v>23</v>
       </c>
@@ -20183,7 +19810,7 @@
         <v>0.36206896551724138</v>
       </c>
     </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:29">
       <c r="A97" s="1">
         <v>24</v>
       </c>
@@ -20267,7 +19894,7 @@
         <v>0.36842105263157893</v>
       </c>
     </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:29">
       <c r="A98" s="1">
         <v>25</v>
       </c>
@@ -20351,7 +19978,7 @@
         <v>0.38095238095238093</v>
       </c>
     </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:29">
       <c r="A99" s="1">
         <v>26</v>
       </c>
@@ -20435,7 +20062,7 @@
         <v>0.39130434782608697</v>
       </c>
     </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:29">
       <c r="A100" s="1">
         <v>27</v>
       </c>
@@ -20519,7 +20146,7 @@
         <v>0.30985915492957744</v>
       </c>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:29">
       <c r="A101" s="1">
         <v>28</v>
       </c>
@@ -20584,7 +20211,7 @@
         <v>0.63636363636363635</v>
       </c>
     </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:29">
       <c r="A102" s="1">
         <v>29</v>
       </c>
@@ -20649,7 +20276,7 @@
         <v>0.63636363636363635</v>
       </c>
     </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:29">
       <c r="A103" s="1">
         <v>30</v>
       </c>
@@ -20714,7 +20341,7 @@
         <v>0.63636363636363635</v>
       </c>
     </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:29">
       <c r="A104" s="1">
         <v>31</v>
       </c>
@@ -20779,7 +20406,7 @@
         <v>0.63636363636363635</v>
       </c>
     </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:29">
       <c r="A105" s="1">
         <v>32</v>
       </c>
@@ -20844,7 +20471,7 @@
         <v>0.72727272727272729</v>
       </c>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:29">
       <c r="A106" s="1">
         <v>33</v>
       </c>
@@ -20909,7 +20536,7 @@
         <v>0.72727272727272729</v>
       </c>
     </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:29">
       <c r="A107" s="1">
         <v>34</v>
       </c>
@@ -20974,7 +20601,7 @@
         <v>0.72727272727272729</v>
       </c>
     </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:29">
       <c r="A108" s="1">
         <v>35</v>
       </c>
@@ -21039,7 +20666,7 @@
         <v>0.72727272727272729</v>
       </c>
     </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:29">
       <c r="A109" s="1">
         <v>36</v>
       </c>
@@ -21104,7 +20731,7 @@
         <v>0.72727272727272729</v>
       </c>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:29">
       <c r="A110" s="1">
         <v>37</v>
       </c>
@@ -21169,7 +20796,7 @@
         <v>0.72727272727272729</v>
       </c>
     </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:29">
       <c r="A111" s="1">
         <v>38</v>
       </c>
@@ -21234,7 +20861,7 @@
         <v>0.81818181818181823</v>
       </c>
     </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:29">
       <c r="A112" s="1">
         <v>39</v>
       </c>
@@ -21299,7 +20926,7 @@
         <v>0.81818181818181823</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:23">
       <c r="A113" s="1">
         <v>40</v>
       </c>
@@ -21364,7 +20991,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:23">
       <c r="A114" s="1">
         <v>41</v>
       </c>
@@ -21429,7 +21056,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:23">
       <c r="A115" s="1">
         <v>42</v>
       </c>
@@ -21494,7 +21121,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:23">
       <c r="A116" s="1">
         <v>43</v>
       </c>
@@ -21559,7 +21186,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:23">
       <c r="A117" s="1">
         <v>44</v>
       </c>
@@ -21624,7 +21251,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:23">
       <c r="A118" s="1">
         <v>45</v>
       </c>
@@ -21689,7 +21316,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:23">
       <c r="A119" s="1">
         <v>46</v>
       </c>
@@ -21754,7 +21381,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:23">
       <c r="A120" s="1">
         <v>47</v>
       </c>
@@ -21819,7 +21446,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:23">
       <c r="A121" s="1">
         <v>48</v>
       </c>
@@ -21884,7 +21511,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:23">
       <c r="A122" s="1">
         <v>49</v>
       </c>
@@ -21949,7 +21576,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:23">
       <c r="A123" s="1">
         <v>50</v>
       </c>
@@ -22014,7 +21641,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:23">
       <c r="A124" s="1">
         <v>51</v>
       </c>
@@ -22079,7 +21706,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:23">
       <c r="A125" s="1">
         <v>52</v>
       </c>
@@ -22144,7 +21771,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:23">
       <c r="A126" s="1">
         <v>53</v>
       </c>
@@ -22209,7 +21836,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:23">
       <c r="A127" s="1">
         <v>54</v>
       </c>
@@ -22274,7 +21901,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:23">
       <c r="A128" s="1">
         <v>55</v>
       </c>
@@ -22339,7 +21966,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:29">
       <c r="A129" s="1">
         <v>56</v>
       </c>
@@ -22404,7 +22031,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:29">
       <c r="A130" s="1">
         <v>57</v>
       </c>
@@ -22469,7 +22096,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:29">
       <c r="A131" s="1">
         <v>58</v>
       </c>
@@ -22534,7 +22161,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:29">
       <c r="A132" s="1">
         <v>59</v>
       </c>
@@ -22599,7 +22226,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:29">
       <c r="A133" s="1">
         <v>60</v>
       </c>
@@ -22664,7 +22291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:29" ht="15">
       <c r="I134" s="5" t="s">
         <v>8</v>
       </c>
@@ -22685,12 +22312,12 @@
         <v>0.18615186949696205</v>
       </c>
     </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:29">
       <c r="A136" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="137" spans="1:29" ht="15" customHeight="1">
       <c r="J137" s="9" t="s">
         <v>7</v>
       </c>
@@ -22718,7 +22345,7 @@
       <c r="AB137" s="9"/>
       <c r="AC137" s="9"/>
     </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:29">
       <c r="A138" s="2" t="s">
         <v>0</v>
       </c>
@@ -22786,7 +22413,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="139" spans="1:29">
       <c r="A139" s="1">
         <v>1</v>
       </c>
@@ -22870,7 +22497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="140" spans="1:29">
       <c r="A140" s="1">
         <v>2</v>
       </c>
@@ -22954,7 +22581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="141" spans="1:29">
       <c r="A141" s="1">
         <v>3</v>
       </c>
@@ -23038,7 +22665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="142" spans="1:29">
       <c r="A142" s="1">
         <v>4</v>
       </c>
@@ -23122,7 +22749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="143" spans="1:29">
       <c r="A143" s="1">
         <v>5</v>
       </c>
@@ -23206,7 +22833,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="144" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="144" spans="1:29">
       <c r="A144" s="1">
         <v>6</v>
       </c>
@@ -23290,7 +22917,7 @@
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="145" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="145" spans="1:29">
       <c r="A145" s="1">
         <v>7</v>
       </c>
@@ -23374,7 +23001,7 @@
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="146" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:29">
       <c r="A146" s="1">
         <v>8</v>
       </c>
@@ -23458,7 +23085,7 @@
         <v>0.78947368421052633</v>
       </c>
     </row>
-    <row r="147" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="147" spans="1:29">
       <c r="A147" s="1">
         <v>9</v>
       </c>
@@ -23542,7 +23169,7 @@
         <v>0.76190476190476186</v>
       </c>
     </row>
-    <row r="148" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="148" spans="1:29">
       <c r="A148" s="1">
         <v>10</v>
       </c>
@@ -23626,7 +23253,7 @@
         <v>0.70370370370370372</v>
       </c>
     </row>
-    <row r="149" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="149" spans="1:29">
       <c r="A149" s="1">
         <v>11</v>
       </c>
@@ -23710,7 +23337,7 @@
         <v>0.68965517241379315</v>
       </c>
     </row>
-    <row r="150" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="150" spans="1:29">
       <c r="A150" s="1">
         <v>12</v>
       </c>
@@ -23775,7 +23402,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="151" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="151" spans="1:29">
       <c r="A151" s="1">
         <v>13</v>
       </c>
@@ -23840,7 +23467,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="152" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:29">
       <c r="A152" s="1">
         <v>14</v>
       </c>
@@ -23905,7 +23532,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="153" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:29">
       <c r="A153" s="1">
         <v>15</v>
       </c>
@@ -23976,7 +23603,7 @@
       <c r="AB153" s="9"/>
       <c r="AC153" s="9"/>
     </row>
-    <row r="154" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="154" spans="1:29">
       <c r="A154" s="1">
         <v>16</v>
       </c>
@@ -24056,7 +23683,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="155" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="155" spans="1:29">
       <c r="A155" s="1">
         <v>17</v>
       </c>
@@ -24140,7 +23767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="156" spans="1:29">
       <c r="A156" s="1">
         <v>18</v>
       </c>
@@ -24224,7 +23851,7 @@
         <v>0.18181818181818182</v>
       </c>
     </row>
-    <row r="157" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="157" spans="1:29">
       <c r="A157" s="1">
         <v>19</v>
       </c>
@@ -24308,7 +23935,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="158" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="158" spans="1:29">
       <c r="A158" s="1">
         <v>20</v>
       </c>
@@ -24392,7 +24019,7 @@
         <v>0.46153846153846151</v>
       </c>
     </row>
-    <row r="159" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="159" spans="1:29">
       <c r="A159" s="1">
         <v>21</v>
       </c>
@@ -24476,7 +24103,7 @@
         <v>0.55384615384615388</v>
       </c>
     </row>
-    <row r="160" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="160" spans="1:29">
       <c r="A160" s="1">
         <v>22</v>
       </c>
@@ -24560,7 +24187,7 @@
         <v>0.63157894736842102</v>
       </c>
     </row>
-    <row r="161" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="161" spans="1:29">
       <c r="A161" s="1">
         <v>23</v>
       </c>
@@ -24644,7 +24271,7 @@
         <v>0.70588235294117641</v>
       </c>
     </row>
-    <row r="162" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="162" spans="1:29">
       <c r="A162" s="1">
         <v>24</v>
       </c>
@@ -24728,7 +24355,7 @@
         <v>0.74204946996466425</v>
       </c>
     </row>
-    <row r="163" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="163" spans="1:29">
       <c r="A163" s="1">
         <v>25</v>
       </c>
@@ -24812,7 +24439,7 @@
         <v>0.78048780487804881</v>
       </c>
     </row>
-    <row r="164" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="164" spans="1:29">
       <c r="A164" s="1">
         <v>26</v>
       </c>
@@ -24896,7 +24523,7 @@
         <v>0.78983833718244822</v>
       </c>
     </row>
-    <row r="165" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="165" spans="1:29">
       <c r="A165" s="1">
         <v>27</v>
       </c>
@@ -24980,7 +24607,7 @@
         <v>0.81632653061224492</v>
       </c>
     </row>
-    <row r="166" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="166" spans="1:29">
       <c r="A166" s="1">
         <v>28</v>
       </c>
@@ -25045,7 +24672,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="167" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="167" spans="1:29">
       <c r="A167" s="1">
         <v>29</v>
       </c>
@@ -25110,7 +24737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="168" spans="1:29">
       <c r="A168" s="1">
         <v>30</v>
       </c>
@@ -25175,7 +24802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="169" spans="1:29" ht="15">
       <c r="I169" s="5" t="s">
         <v>8</v>
       </c>
@@ -25196,12 +24823,12 @@
         <v>0.81775673128684445</v>
       </c>
     </row>
-    <row r="171" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="171" spans="1:29">
       <c r="E171" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="172" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="172" spans="1:29" ht="15">
       <c r="I172" s="6" t="s">
         <v>13</v>
       </c>
@@ -25222,17 +24849,17 @@
         <v>0.6252994716035124</v>
       </c>
     </row>
-    <row r="173" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="173" spans="1:29">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
     </row>
-    <row r="174" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="174" spans="1:29">
       <c r="A174" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="175" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="175" spans="1:29">
       <c r="F175" s="9" t="s">
         <v>10</v>
       </c>
@@ -25240,7 +24867,7 @@
       <c r="H175" s="9"/>
       <c r="I175" s="9"/>
     </row>
-    <row r="176" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="176" spans="1:29">
       <c r="E176" s="3" t="s">
         <v>11</v>
       </c>
@@ -25257,7 +24884,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="177" spans="4:11" x14ac:dyDescent="0.5">
+    <row r="177" spans="4:11">
       <c r="E177" s="4">
         <v>0</v>
       </c>
@@ -25280,7 +24907,7 @@
       <c r="J177" s="9"/>
       <c r="K177" s="9"/>
     </row>
-    <row r="178" spans="4:11" x14ac:dyDescent="0.5">
+    <row r="178" spans="4:11">
       <c r="E178" s="4">
         <v>0.1</v>
       </c>
@@ -25303,7 +24930,7 @@
       <c r="J178" s="2"/>
       <c r="K178" s="2"/>
     </row>
-    <row r="179" spans="4:11" x14ac:dyDescent="0.5">
+    <row r="179" spans="4:11">
       <c r="E179" s="4">
         <v>0.2</v>
       </c>
@@ -25324,7 +24951,7 @@
         <v>0.8214285714285714</v>
       </c>
     </row>
-    <row r="180" spans="4:11" x14ac:dyDescent="0.5">
+    <row r="180" spans="4:11">
       <c r="E180" s="4">
         <v>0.3</v>
       </c>
@@ -25345,7 +24972,7 @@
         <v>0.8214285714285714</v>
       </c>
     </row>
-    <row r="181" spans="4:11" x14ac:dyDescent="0.5">
+    <row r="181" spans="4:11">
       <c r="E181" s="4">
         <v>0.4</v>
       </c>
@@ -25366,7 +24993,7 @@
         <v>0.79642857142857137</v>
       </c>
     </row>
-    <row r="182" spans="4:11" x14ac:dyDescent="0.5">
+    <row r="182" spans="4:11">
       <c r="E182" s="4">
         <v>0.5</v>
       </c>
@@ -25387,7 +25014,7 @@
         <v>0.66552197802197799</v>
       </c>
     </row>
-    <row r="183" spans="4:11" x14ac:dyDescent="0.5">
+    <row r="183" spans="4:11">
       <c r="E183" s="4">
         <v>0.6</v>
       </c>
@@ -25408,7 +25035,7 @@
         <v>0.6194366635543106</v>
       </c>
     </row>
-    <row r="184" spans="4:11" x14ac:dyDescent="0.5">
+    <row r="184" spans="4:11">
       <c r="E184" s="4">
         <v>0.7</v>
       </c>
@@ -25429,7 +25056,7 @@
         <v>0.59633458646616533</v>
       </c>
     </row>
-    <row r="185" spans="4:11" x14ac:dyDescent="0.5">
+    <row r="185" spans="4:11">
       <c r="E185" s="4">
         <v>0.8</v>
       </c>
@@ -25450,7 +25077,7 @@
         <v>0.57809934318555012</v>
       </c>
     </row>
-    <row r="186" spans="4:11" x14ac:dyDescent="0.5">
+    <row r="186" spans="4:11">
       <c r="E186" s="4">
         <v>0.9</v>
       </c>
@@ -25471,7 +25098,7 @@
         <v>0.54843918852539542</v>
       </c>
     </row>
-    <row r="187" spans="4:11" x14ac:dyDescent="0.5">
+    <row r="187" spans="4:11">
       <c r="E187" s="4">
         <v>1</v>
       </c>
@@ -25492,12 +25119,12 @@
         <v>0.51997126436781604</v>
       </c>
     </row>
-    <row r="189" spans="4:11" x14ac:dyDescent="0.5">
+    <row r="189" spans="4:11">
       <c r="D189" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="191" spans="4:11" x14ac:dyDescent="0.5">
+    <row r="191" spans="4:11">
       <c r="F191" s="9" t="s">
         <v>10</v>
       </c>
@@ -25505,7 +25132,7 @@
       <c r="H191" s="9"/>
       <c r="I191" s="9"/>
     </row>
-    <row r="192" spans="4:11" x14ac:dyDescent="0.5">
+    <row r="192" spans="4:11">
       <c r="E192" s="3" t="s">
         <v>11</v>
       </c>
@@ -25522,7 +25149,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="193" spans="5:9" x14ac:dyDescent="0.5">
+    <row r="193" spans="4:9">
       <c r="E193" s="4">
         <v>0</v>
       </c>
@@ -25543,7 +25170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="5:9" x14ac:dyDescent="0.5">
+    <row r="194" spans="4:9">
       <c r="E194" s="4">
         <v>0.1</v>
       </c>
@@ -25564,7 +25191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="5:9" x14ac:dyDescent="0.5">
+    <row r="195" spans="4:9">
       <c r="E195" s="4">
         <v>0.2</v>
       </c>
@@ -25585,7 +25212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="5:9" x14ac:dyDescent="0.5">
+    <row r="196" spans="4:9">
       <c r="E196" s="4">
         <v>0.3</v>
       </c>
@@ -25606,7 +25233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="5:9" x14ac:dyDescent="0.5">
+    <row r="197" spans="4:9">
       <c r="E197" s="4">
         <v>0.4</v>
       </c>
@@ -25627,7 +25254,7 @@
         <v>0.96666666666666667</v>
       </c>
     </row>
-    <row r="198" spans="5:9" x14ac:dyDescent="0.5">
+    <row r="198" spans="4:9">
       <c r="E198" s="4">
         <v>0.5</v>
       </c>
@@ -25648,7 +25275,7 @@
         <v>0.79212454212454209</v>
       </c>
     </row>
-    <row r="199" spans="5:9" x14ac:dyDescent="0.5">
+    <row r="199" spans="4:9">
       <c r="E199" s="4">
         <v>0.6</v>
       </c>
@@ -25669,7 +25296,7 @@
         <v>0.73949579831932777</v>
       </c>
     </row>
-    <row r="200" spans="5:9" x14ac:dyDescent="0.5">
+    <row r="200" spans="4:9">
       <c r="E200" s="4">
         <v>0.7</v>
       </c>
@@ -25690,7 +25317,7 @@
         <v>0.71177944862155373</v>
       </c>
     </row>
-    <row r="201" spans="5:9" x14ac:dyDescent="0.5">
+    <row r="201" spans="4:9">
       <c r="E201" s="4">
         <v>0.8</v>
       </c>
@@ -25711,7 +25338,7 @@
         <v>0.68746579091406679</v>
       </c>
     </row>
-    <row r="202" spans="5:9" x14ac:dyDescent="0.5">
+    <row r="202" spans="4:9">
       <c r="E202" s="4">
         <v>0.9</v>
       </c>
@@ -25732,7 +25359,7 @@
         <v>0.64791891803386059</v>
       </c>
     </row>
-    <row r="203" spans="5:9" x14ac:dyDescent="0.5">
+    <row r="203" spans="4:9">
       <c r="E203" s="4">
         <v>1</v>
       </c>
@@ -25753,42 +25380,50 @@
         <v>0.63218390804597702</v>
       </c>
     </row>
-    <row r="204" spans="5:9" x14ac:dyDescent="0.5">
+    <row r="204" spans="4:9">
       <c r="E204" s="4"/>
     </row>
-    <row r="205" spans="5:9" x14ac:dyDescent="0.5">
+    <row r="205" spans="4:9">
       <c r="E205" s="4"/>
     </row>
-    <row r="206" spans="5:9" x14ac:dyDescent="0.5">
+    <row r="206" spans="4:9">
       <c r="E206" s="4"/>
     </row>
-    <row r="207" spans="5:9" x14ac:dyDescent="0.5">
-      <c r="E207" s="4"/>
+    <row r="207" spans="4:9" ht="15">
+      <c r="D207" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E207" s="10">
+        <f>AVERAGE(J169,J69,J34)</f>
+        <v>0.55669508166485171</v>
+      </c>
+      <c r="F207" s="10">
+        <f t="shared" ref="F207:H207" si="77">AVERAGE(K169,K69,K34)</f>
+        <v>0.64423085921344969</v>
+      </c>
+      <c r="G207" s="10">
+        <f t="shared" si="77"/>
+        <v>0.56058863107380252</v>
+      </c>
+      <c r="H207" s="10">
+        <f t="shared" si="77"/>
+        <v>0.77168200563902911</v>
+      </c>
     </row>
-    <row r="208" spans="5:9" x14ac:dyDescent="0.5">
+    <row r="208" spans="4:9">
       <c r="E208" s="4"/>
     </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="209" spans="5:5">
       <c r="E209" s="4"/>
     </row>
-    <row r="210" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="210" spans="5:5">
       <c r="E210" s="4"/>
     </row>
-    <row r="211" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="211" spans="5:5">
       <c r="E211" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="F191:I191"/>
-    <mergeCell ref="Z137:AC137"/>
-    <mergeCell ref="F175:I175"/>
-    <mergeCell ref="Z153:AC153"/>
-    <mergeCell ref="Z88:AC88"/>
-    <mergeCell ref="Z53:AC53"/>
-    <mergeCell ref="O137:R137"/>
-    <mergeCell ref="T137:W137"/>
-    <mergeCell ref="J177:K177"/>
-    <mergeCell ref="Z18:AC18"/>
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="T2:W2"/>
     <mergeCell ref="O2:R2"/>
@@ -25797,11 +25432,21 @@
     <mergeCell ref="O37:R37"/>
     <mergeCell ref="T37:W37"/>
     <mergeCell ref="Z37:AC37"/>
+    <mergeCell ref="Z53:AC53"/>
+    <mergeCell ref="O137:R137"/>
+    <mergeCell ref="T137:W137"/>
+    <mergeCell ref="J177:K177"/>
+    <mergeCell ref="Z18:AC18"/>
     <mergeCell ref="J72:M72"/>
     <mergeCell ref="O72:R72"/>
     <mergeCell ref="T72:W72"/>
     <mergeCell ref="Z72:AC72"/>
     <mergeCell ref="J137:M137"/>
+    <mergeCell ref="F191:I191"/>
+    <mergeCell ref="Z137:AC137"/>
+    <mergeCell ref="F175:I175"/>
+    <mergeCell ref="Z153:AC153"/>
+    <mergeCell ref="Z88:AC88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
excel fix and something else
</commit_message>
<xml_diff>
--- a/solr/EvaluationM3.xlsx
+++ b/solr/EvaluationM3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\PRI\solr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedrofonseca/Documents/FEUP/PRI/PRI/solr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4587DEF9-1E4A-4A6B-94FA-6E6E524F8DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025F160A-AEAD-444B-9E02-AE2C50557AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1F5A3B19-910C-4A1F-9359-A2D6231D0330}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="44660" windowHeight="23720" xr2:uid="{1F5A3B19-910C-4A1F-9359-A2D6231D0330}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -255,7 +255,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1218,7 +1218,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -1324,7 +1324,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -1365,7 +1365,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1395,7 +1395,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1409,7 +1409,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2930,7 +2930,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -3036,7 +3036,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -3077,7 +3077,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3107,7 +3107,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3121,7 +3121,7 @@
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3719,7 +3719,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -3825,7 +3825,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -3866,7 +3866,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3896,7 +3896,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3910,7 +3910,7 @@
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4521,7 +4521,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -4627,7 +4627,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -4668,7 +4668,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4698,7 +4698,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4712,7 +4712,7 @@
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5310,7 +5310,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -5416,7 +5416,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -5457,7 +5457,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5487,7 +5487,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5501,7 +5501,7 @@
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6099,7 +6099,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -6205,7 +6205,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -6246,7 +6246,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6276,7 +6276,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6290,7 +6290,7 @@
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7811,7 +7811,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -7917,7 +7917,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -7958,7 +7958,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7988,7 +7988,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8002,7 +8002,7 @@
 <file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -8384,59 +8384,47 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AF$139:$AF$149</c:f>
+              <c:f>Sheet1!$AF$174:$AF$184</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.42857142857142855</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.9</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8571428571428571</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8571428571428571</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.78947368421052633</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.76190476190476186</c:v>
+                  <c:v>0.34782608695652173</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.70370370370370372</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.68965517241379315</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8600,7 +8588,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -8706,7 +8694,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -8747,7 +8735,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -8777,7 +8765,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8791,7 +8779,7 @@
 <file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -9402,7 +9390,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -9508,7 +9496,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -9549,7 +9537,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9579,7 +9567,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9593,7 +9581,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -10191,7 +10179,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -10297,7 +10285,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -10338,7 +10326,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -10368,7 +10356,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10382,7 +10370,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -10993,7 +10981,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -11099,7 +11087,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -11140,7 +11128,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -11170,7 +11158,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11184,7 +11172,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -12147,7 +12135,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -12253,7 +12241,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -12294,7 +12282,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -12324,7 +12312,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -12338,7 +12326,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -12936,7 +12924,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -13042,7 +13030,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -13083,7 +13071,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -13113,7 +13101,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -13127,7 +13115,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -13738,7 +13726,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -13844,7 +13832,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -13885,7 +13873,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -13915,7 +13903,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -13929,7 +13917,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -15900,7 +15888,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -16006,7 +15994,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -16047,7 +16035,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -16077,7 +16065,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -16091,7 +16079,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -16689,7 +16677,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -16795,7 +16783,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -16836,7 +16824,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -16866,7 +16854,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -16880,7 +16868,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -17491,7 +17479,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1331152447"/>
@@ -17597,7 +17585,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1361606489"/>
@@ -17638,7 +17626,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -17668,7 +17656,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -18777,21 +18765,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90E2CE5-2754-4DEC-9740-5E5101C42739}">
   <dimension ref="A1:HW246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H206" sqref="H206"/>
+    <sheetView tabSelected="1" topLeftCell="C175" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N207" sqref="N207"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="14" width="9.140625" style="1"/>
-    <col min="15" max="15" width="9.140625" style="1" customWidth="1"/>
-    <col min="16" max="25" width="9.140625" style="1"/>
-    <col min="26" max="26" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="9.140625" style="1"/>
-    <col min="29" max="29" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="5" width="9.1640625" style="1"/>
+    <col min="6" max="6" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="14" width="9.1640625" style="1"/>
+    <col min="15" max="15" width="9.1640625" style="1" customWidth="1"/>
+    <col min="16" max="25" width="9.1640625" style="1"/>
+    <col min="26" max="26" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="9.1640625" style="1"/>
+    <col min="29" max="29" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -18802,7 +18790,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="15">
+    <row r="2" spans="1:33">
       <c r="J2" s="11" t="s">
         <v>7</v>
       </c>
@@ -21852,7 +21840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:33" ht="15">
+    <row r="34" spans="1:33">
       <c r="I34" s="5" t="s">
         <v>8</v>
       </c>
@@ -24928,7 +24916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:33" ht="15">
+    <row r="69" spans="1:33">
       <c r="I69" s="5" t="s">
         <v>8</v>
       </c>
@@ -30404,7 +30392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:33" ht="15">
+    <row r="134" spans="1:33">
       <c r="I134" s="5" t="s">
         <v>8</v>
       </c>
@@ -33480,7 +33468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:231" ht="15">
+    <row r="169" spans="1:231">
       <c r="I169" s="5" t="s">
         <v>8</v>
       </c>
@@ -33510,7 +33498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="171" spans="1:231" ht="15">
+    <row r="171" spans="1:231">
       <c r="A171" s="1" t="s">
         <v>22</v>
       </c>
@@ -33545,7 +33533,7 @@
       <c r="HV171" s="11"/>
       <c r="HW171" s="11"/>
     </row>
-    <row r="172" spans="1:231" ht="15">
+    <row r="172" spans="1:231">
       <c r="J172" s="11" t="s">
         <v>7</v>
       </c>
@@ -38925,7 +38913,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row r="203" spans="1:230" ht="15">
+    <row r="203" spans="1:230">
       <c r="A203" s="1">
         <v>30</v>
       </c>
@@ -39025,7 +39013,7 @@
       </c>
       <c r="HD203" s="5"/>
     </row>
-    <row r="204" spans="1:230" ht="15">
+    <row r="204" spans="1:230">
       <c r="I204" s="5" t="s">
         <v>8</v>
       </c>
@@ -39050,7 +39038,7 @@
         <v>0.66885774136247977</v>
       </c>
     </row>
-    <row r="207" spans="1:230" ht="15">
+    <row r="207" spans="1:230">
       <c r="E207" s="1" t="s">
         <v>16</v>
       </c>
@@ -39712,7 +39700,7 @@
     <row r="241" spans="4:9">
       <c r="E241" s="4"/>
     </row>
-    <row r="242" spans="4:9" ht="15">
+    <row r="242" spans="4:9">
       <c r="D242" s="6" t="s">
         <v>13</v>
       </c>
@@ -39751,6 +39739,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="AC188:AG188"/>
+    <mergeCell ref="GZ171:HD171"/>
+    <mergeCell ref="HF171:HJ171"/>
+    <mergeCell ref="HL171:HP171"/>
+    <mergeCell ref="AC2:AG2"/>
+    <mergeCell ref="AC137:AG137"/>
+    <mergeCell ref="AC88:AG88"/>
+    <mergeCell ref="AC153:AG153"/>
+    <mergeCell ref="AC72:AG72"/>
+    <mergeCell ref="AC37:AG37"/>
+    <mergeCell ref="V37:Z37"/>
+    <mergeCell ref="HS171:HW171"/>
+    <mergeCell ref="HS187:HW187"/>
+    <mergeCell ref="AC53:AG53"/>
+    <mergeCell ref="AC18:AG18"/>
+    <mergeCell ref="AC172:AG172"/>
     <mergeCell ref="J2:N2"/>
     <mergeCell ref="V2:Z2"/>
     <mergeCell ref="P2:T2"/>
@@ -39767,22 +39771,6 @@
     <mergeCell ref="J72:N72"/>
     <mergeCell ref="J37:N37"/>
     <mergeCell ref="P37:T37"/>
-    <mergeCell ref="V37:Z37"/>
-    <mergeCell ref="HS171:HW171"/>
-    <mergeCell ref="HS187:HW187"/>
-    <mergeCell ref="AC53:AG53"/>
-    <mergeCell ref="AC18:AG18"/>
-    <mergeCell ref="AC2:AG2"/>
-    <mergeCell ref="AC137:AG137"/>
-    <mergeCell ref="AC88:AG88"/>
-    <mergeCell ref="AC153:AG153"/>
-    <mergeCell ref="AC72:AG72"/>
-    <mergeCell ref="AC37:AG37"/>
-    <mergeCell ref="AC172:AG172"/>
-    <mergeCell ref="AC188:AG188"/>
-    <mergeCell ref="GZ171:HD171"/>
-    <mergeCell ref="HF171:HJ171"/>
-    <mergeCell ref="HL171:HP171"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>